<commit_message>
Fix value of SCALE pot
</commit_message>
<xml_diff>
--- a/dws-BOM.xlsx
+++ b/dws-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -82,10 +82,13 @@
     <t xml:space="preserve">SCALE1</t>
   </si>
   <si>
+    <t xml:space="preserve">B10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLOPE1</t>
+  </si>
+  <si>
     <t xml:space="preserve">B100k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLOPE1</t>
   </si>
   <si>
     <t xml:space="preserve">Q1, Q2</t>
@@ -181,6 +184,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -202,6 +206,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -279,14 +284,14 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -408,7 +413,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,10 +421,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,10 +432,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,10 +443,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,10 +454,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,10 +465,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,10 +476,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,10 +487,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,10 +498,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,10 +509,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,10 +520,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,10 +531,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,10 +542,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -548,10 +553,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,10 +564,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>